<commit_message>
first commit to branch
</commit_message>
<xml_diff>
--- a/recruit_info.xlsx
+++ b/recruit_info.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6e4dedc551d01c3d/AKP/Projects/autoHR-main/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rahul Kalubowila\OneDrive\AKP\Projects\autoHR-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{F1A185DD-B1D5-43B6-BE0A-7D1A8DEC39B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DEBDE308-E0A8-4BBA-978E-425343216E3A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FC32D9-A8E6-4AAB-AF01-F1383992F57F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7959ACFA-E93F-434B-9017-C7745B76C140}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>name</t>
   </si>
@@ -408,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB18F163-0929-4DCF-9063-B9289952D575}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,42 +440,31 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{D5DEFC44-38FC-4502-8D65-408BB6045D38}"/>
-    <hyperlink ref="C3:C4" r:id="rId2" display="lankadinee@gmail.com" xr:uid="{FEAEA79D-40F2-4CC9-AD06-653CC5C72CF4}"/>
-    <hyperlink ref="C5" r:id="rId3" xr:uid="{29C92410-0798-4B07-8AF6-FD1526ECC99A}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{29C92410-0798-4B07-8AF6-FD1526ECC99A}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{BEF303ED-29CA-4D59-B9E6-1135CB11E80C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>